<commit_message>
Add team name and project repo link
</commit_message>
<xml_diff>
--- a/Security Task Team Information.xlsx
+++ b/Security Task Team Information.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makka\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D07611-060B-4F02-845B-507462F4CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="12084" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>لينك ال repo</t>
   </si>
@@ -56,6 +50,9 @@
     <t>اسم الفرد السادس</t>
   </si>
   <si>
+    <t>https://github.com/AbdallahHikal/Steganography.git</t>
+  </si>
+  <si>
     <t xml:space="preserve">احمد خالد محمد </t>
   </si>
   <si>
@@ -68,36 +65,51 @@
     <t>روان زينهم عبدالعزيز</t>
   </si>
   <si>
+    <t>عبدالرحمن علاء الدين عبدالمنعم</t>
+  </si>
+  <si>
     <t>عبدالله محمد خالد عبدالباسط</t>
   </si>
   <si>
-    <t>عبدالرحمن علاء الدين عبدالمنعم</t>
-  </si>
-  <si>
-    <t>https://github.com/AbdallahHikal/Steganography.git</t>
+    <t>https://github.com/AbdoFattou7/Streaming_app.git</t>
+  </si>
+  <si>
+    <t>عبدالرحمن احمد فتوح</t>
+  </si>
+  <si>
+    <t>احمد محمد احمد محمد</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -105,10 +117,154 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,8 +277,194 @@
         <bgColor rgb="FF4A86E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -130,34 +472,316 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -355,32 +979,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="C9:F9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.712962962963" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="55.1388888888889" customWidth="1"/>
+    <col min="2" max="3" width="19.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="22.1388888888889" customWidth="1"/>
+    <col min="5" max="5" width="21.1388888888889" customWidth="1"/>
+    <col min="6" max="6" width="25.8518518518519" customWidth="1"/>
+    <col min="7" max="7" width="31.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,33 +1027,45 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" customHeight="1" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{03467FED-0208-4A25-A788-A9E8AD3C9445}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://github.com/AbdallahHikal/Steganography.git"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>